<commit_message>
Process data, make figs
</commit_message>
<xml_diff>
--- a/Impedance_Analyzer_V2_KiCAD/Impedance_Analyzer_V2_MouserBOM.xlsx
+++ b/Impedance_Analyzer_V2_KiCAD/Impedance_Analyzer_V2_MouserBOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/588f4a293b9f2941/Documents/GitHub/Simple_Impedance_Analyzer/Impedance_Analyzer_V2_KiCAD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elima\OneDrive\Documents\GitHub\Simple_Impedance_Analyzer\Impedance_Analyzer_V2_KiCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="8544"/>
   </bookViews>
   <sheets>
     <sheet name="Impedance_Analyzer_V2" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>Comment</t>
   </si>
@@ -234,15 +234,9 @@
     <t>Martinos:SIP-2W-7</t>
   </si>
   <si>
-    <t>LM358</t>
-  </si>
-  <si>
     <t>U1,U2</t>
   </si>
   <si>
-    <t>INA129</t>
-  </si>
-  <si>
     <t>U3,U4</t>
   </si>
   <si>
@@ -301,6 +295,21 @@
   </si>
   <si>
     <t>71-TNPW1206100RBYEN</t>
+  </si>
+  <si>
+    <t>OPA2830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shorting pins </t>
+  </si>
+  <si>
+    <t>571-28815452</t>
+  </si>
+  <si>
+    <t>INA121</t>
+  </si>
+  <si>
+    <t>Order 10+</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1177,7 +1186,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,7 +1222,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1238,7 +1247,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1252,7 +1261,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1277,7 +1286,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1335,7 +1344,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1349,7 +1358,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1385,7 +1394,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1399,7 +1408,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1446,7 +1455,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1482,7 +1491,7 @@
         <v>59</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1496,46 +1505,57 @@
         <v>70</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
         <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>72</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
       </c>
-      <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" t="s">
-        <v>75</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
         <v>76</v>
       </c>
-      <c r="B31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" t="s">
-        <v>78</v>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>